<commit_message>
Ajout des tableaux corrige et affichage des colonnes vides
</commit_message>
<xml_diff>
--- a/Donnees/Statisiques Environnementales et de la  gouvernace/Gouvernance/IND-Gouvernace 14-08-2025xlsb.xlsx
+++ b/Donnees/Statisiques Environnementales et de la  gouvernace/Gouvernance/IND-Gouvernace 14-08-2025xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Ansade_Project\Donnees\Statisiques Environnementales et de la  gouvernace\Gouvernance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansad\OneDrive\Desktop\Gouvernance\Mon Travail\Annuaires et tableaux de service\Telech site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40D8EA57-E18C-45FF-BA1F-D4C0BDD7AED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C29DEA1-5AF3-4A9F-8172-E05F617EC597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TSN1" sheetId="4" r:id="rId1"/>
@@ -33,19 +33,29 @@
     <sheet name="TDH3" sheetId="27" r:id="rId18"/>
     <sheet name="TDH4" sheetId="28" r:id="rId19"/>
     <sheet name="TDH5" sheetId="29" r:id="rId20"/>
-    <sheet name="Feuil1" sheetId="30" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="177">
   <si>
     <t>Source: https://data.unhcr.org/fr/country/mrt</t>
   </si>
@@ -83,27 +93,9 @@
     <t>Source: Direction Générale de la Sureté Nationale</t>
   </si>
   <si>
-    <t>Tableau TSN2: L'évolution du nombre de demandeurs d'asile par sexe 2019-2024</t>
-  </si>
-  <si>
-    <t>Tableau TSN3 : L'évolution du nombre de demandeurs d'asile en Mauritanie par groupe d'age 2019-2024</t>
-  </si>
-  <si>
-    <t>Tableau TSN4 : L'évolution du nombre de réfugiés en Mauritanie par sexe 2019-2024</t>
-  </si>
-  <si>
-    <t>Tableau TSN5 : L'évolution du nombre de réfugiés en Mauritanie par groupe d'age, 2019-2024</t>
-  </si>
-  <si>
     <t>Nombre de crime meurtrier</t>
   </si>
   <si>
-    <t>Taux d'homicide(pour 100000 habitants)</t>
-  </si>
-  <si>
-    <t>Tableau 4.8:  L'évolution du taux d'homicide en Mauritanie selon la Wilaya 2020 -2024</t>
-  </si>
-  <si>
     <t>Wilaya</t>
   </si>
   <si>
@@ -149,9 +141,6 @@
     <t>Enssemble</t>
   </si>
   <si>
-    <t>Tableau TPS1:  L'évolution de taux d'homicide en Mauritanie 2000-2024</t>
-  </si>
-  <si>
     <t>Source: Ministére de la Justice/ Direction de Prison</t>
   </si>
   <si>
@@ -188,9 +177,6 @@
     <t xml:space="preserve">Pourcentage d'éfficacité </t>
   </si>
   <si>
-    <t>Nombre total de détenus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nombre de personnes en détention provisoire  </t>
   </si>
   <si>
@@ -219,30 +205,6 @@
   </si>
   <si>
     <t>Nombre de femmes détenues</t>
-  </si>
-  <si>
-    <t>Tableau SJ1:  Population carcérale totale en Mauritanie par sexe 2019 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ2:  Repartition des detenus par sexe et par prison en Mauritanie, 2019 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau  TSJ3:  Repartition des detenus selon la catégories d'âge et par prison principale, 2019 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ4:  Repartition des detenus par nationalité et prison 2020 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ5:  Repartition des detenus par type de détention et prison 2019 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ6:  Efficacité du système judiciaire en Mauritanie 2010-2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ7: Evolution duTaux d'occupastion par  prison 2020 - 2024</t>
-  </si>
-  <si>
-    <t>Tableau TSJ8:  Pourcentage de la population féminine carcérale  en Mauritanie 2010-2024</t>
   </si>
   <si>
     <t>Détenus</t>
@@ -273,15 +235,6 @@
     <t>Nombre d'inscrits</t>
   </si>
   <si>
-    <t>Pourcentage de femmes</t>
-  </si>
-  <si>
-    <t>Nombre de femme</t>
-  </si>
-  <si>
-    <t>Nombre total de siège</t>
-  </si>
-  <si>
     <t>Sièges</t>
   </si>
   <si>
@@ -300,33 +253,12 @@
     <t>Nombre de sièges</t>
   </si>
   <si>
-    <t>Nombre d'inscrit</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Année d'élection   </t>
   </si>
   <si>
     <t xml:space="preserve">Année d'élection   </t>
   </si>
   <si>
-    <t>Tableau TDH1 :Résultats des élections présidentielles en Mauritanie 2014-2024</t>
-  </si>
-  <si>
-    <t>Tableau TDH2: Pourcentage de femmes dans le parlement Mauritanien 2013 - 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tableau TDH3: Taux de participation au élections Législatives en Mauritanie 2013 - 2023 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tableau TDH4: Taux de participation au élections Communales en Mauritanie 2013 - 2023 </t>
-  </si>
-  <si>
-    <t>Tableau TDH5: Participation aux élections régionales 2018 - 2023</t>
-  </si>
-  <si>
-    <t>Tableau TSN1:  Evolution de nombre de refigés maliens enregistrés dans le camp d'Mbera, 2019-2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">  2020~Nombre de crime meurtrier</t>
   </si>
   <si>
@@ -580,6 +512,81 @@
   </si>
   <si>
     <t>Année d'élection~ 2023</t>
+  </si>
+  <si>
+    <t>Tableau TSN2: L'évolution du nombre de demandeurs d'asile en Mauritanie par sexe durant la période 2019-2024</t>
+  </si>
+  <si>
+    <t>Tableau TSN1:  Evolution du nombre des refugés maliens enregistrés dans le camp de M'bera durant la période  2019-2024</t>
+  </si>
+  <si>
+    <t>Tableau TSN3 : L'évolution du nombre de demandeurs d'asile en Mauritanie par groupe d'age durant la période 2019-2024</t>
+  </si>
+  <si>
+    <t>Tableau TSN4 : L'évolution du nombre de réfugés en Mauritanie par sexe durant la période 2019-2024</t>
+  </si>
+  <si>
+    <t>Tableau TSN5 : L'évolution du nombre de réfugés en Mauritanie par groupe d'age durant la période 2019-2024</t>
+  </si>
+  <si>
+    <t>Tableau TPS1:  L'évolution du taux d'homicide en Mauritanie durant la période 2000-2024</t>
+  </si>
+  <si>
+    <t>Taux d'homicide (pour 100000 habitants)</t>
+  </si>
+  <si>
+    <t>Tableau 4.8:  L'évolution du taux d'homicide en Mauritanie selon la Wilaya durant la période 2020 -2024</t>
+  </si>
+  <si>
+    <t>Tableau SJ1:  Population carcérale totale en Mauritanie par sexe durant la période 2019 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau TSJ2:  Repartition des detenus par sexe et prison en Mauritanie durant la période 2019 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau  TSJ3:  Repartition des detenus selon les catégories d'âge et par prison principale durant la période 2019 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau TSJ4:  Repartition des detenus par nationalité et prison durant la période 2020 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau TSJ5:  Repartition des detenus par type de détention et prison  durant la période 2019 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau TSJ6:  Efficacité du système judiciaire en Mauritanie durant la période 2010-2024</t>
+  </si>
+  <si>
+    <t>Nombre totale de détenus</t>
+  </si>
+  <si>
+    <t>Tableau TSJ7: Evolution du taux d'occupation par  prison durant la période 2020 - 2024</t>
+  </si>
+  <si>
+    <t>Tableau TSJ8:  Pourcentage de la population féminine carcérale  en Mauritanie durant la période 2010-2024</t>
+  </si>
+  <si>
+    <t>Tableau TDH1 :Résultats des élections présidentielles en Mauritanie duant la période 2014-2024</t>
+  </si>
+  <si>
+    <t>Tableau TDH2: Pourcentage de femmes dans le parlement Mauritanien durant la période 2013 - 2023</t>
+  </si>
+  <si>
+    <t>Nombre totale de siège</t>
+  </si>
+  <si>
+    <t>Nombre des femmes</t>
+  </si>
+  <si>
+    <t>Pourcentage des femmes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau TDH3: Taux de participation aux élections législatives en Mauritanie  durant la période 2013 - 2023 </t>
+  </si>
+  <si>
+    <t>Tableau TDH5: Participation aux élections régionales durant la période  2018 - 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau TDH4: Taux de participation aux élections communales en Mauritanie durant la période 2013 - 2023 </t>
   </si>
 </sst>
 </file>
@@ -1887,17 +1894,17 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27.65" customHeight="1" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:8" ht="30" thickBot="1" x14ac:dyDescent="1">
       <c r="A1" s="154" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="B1" s="154"/>
       <c r="C1" s="154"/>
@@ -1907,7 +1914,7 @@
       <c r="G1" s="154"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1930,7 +1937,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" ht="27.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1953,7 +1960,7 @@
         <v>116055</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1975,22 +1982,20 @@
   </sheetPr>
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="18" width="11.109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="11.08984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:20" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="33" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -2011,68 +2016,68 @@
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
     </row>
-    <row r="2" spans="1:20" ht="79.2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:20" ht="81" x14ac:dyDescent="0.9">
       <c r="A2" s="140" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="110" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C2" s="111" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D2" s="110" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="29" t="s">
+      <c r="M2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="63" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="O2" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>139</v>
-      </c>
       <c r="R2" s="63" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="S2" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A3" s="60" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="112">
         <v>760</v>
@@ -2086,7 +2091,7 @@
         <v>609</v>
       </c>
       <c r="F3" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G3" s="61">
         <v>609</v>
@@ -2095,7 +2100,7 @@
         <v>935</v>
       </c>
       <c r="I3" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J3" s="61">
         <v>935</v>
@@ -2104,7 +2109,7 @@
         <v>1039</v>
       </c>
       <c r="L3" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M3" s="61">
         <v>1039</v>
@@ -2113,7 +2118,7 @@
         <v>1017</v>
       </c>
       <c r="O3" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P3" s="61">
         <v>1017</v>
@@ -2128,9 +2133,9 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A4" s="60" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B4" s="112">
         <v>102</v>
@@ -2144,7 +2149,7 @@
         <v>84</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G4" s="61">
         <v>84</v>
@@ -2153,7 +2158,7 @@
         <v>108</v>
       </c>
       <c r="I4" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J4" s="61">
         <v>108</v>
@@ -2162,7 +2167,7 @@
         <v>115</v>
       </c>
       <c r="L4" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M4" s="61">
         <v>115</v>
@@ -2171,7 +2176,7 @@
         <v>108</v>
       </c>
       <c r="O4" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P4" s="61">
         <v>108</v>
@@ -2186,9 +2191,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A5" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="112">
         <v>413</v>
@@ -2222,7 +2227,7 @@
         <v>383</v>
       </c>
       <c r="L5" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M5" s="61">
         <v>383</v>
@@ -2231,7 +2236,7 @@
         <v>312</v>
       </c>
       <c r="O5" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P5" s="61">
         <v>312</v>
@@ -2246,9 +2251,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A6" s="60" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B6" s="112">
         <v>589</v>
@@ -2262,7 +2267,7 @@
         <v>295</v>
       </c>
       <c r="F6" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G6" s="61">
         <v>295</v>
@@ -2271,7 +2276,7 @@
         <v>444</v>
       </c>
       <c r="I6" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J6" s="61">
         <v>444</v>
@@ -2304,9 +2309,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.9">
       <c r="A7" s="60" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B7" s="112">
         <v>24</v>
@@ -2331,7 +2336,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J7" s="61">
         <v>44</v>
@@ -2340,7 +2345,7 @@
         <v>41</v>
       </c>
       <c r="L7" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M7" s="61">
         <v>41</v>
@@ -2349,7 +2354,7 @@
         <v>35</v>
       </c>
       <c r="O7" s="66" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P7" s="61">
         <v>35</v>
@@ -2364,9 +2369,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:20" ht="15.65" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A8" s="50" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
@@ -2402,18 +2407,18 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="16" width="16.21875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="16" width="16.1796875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30.6" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:16" ht="30" thickBot="1" x14ac:dyDescent="1">
       <c r="A1" s="55" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -2431,89 +2436,89 @@
       <c r="O1" s="55"/>
       <c r="P1" s="55"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A2" s="141" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="159" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="C2" s="160"/>
       <c r="D2" s="161"/>
       <c r="E2" s="159" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="F2" s="160"/>
       <c r="G2" s="161"/>
       <c r="H2" s="156" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="I2" s="157"/>
       <c r="J2" s="158"/>
       <c r="K2" s="156" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="L2" s="157"/>
       <c r="M2" s="158"/>
       <c r="N2" s="162" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="O2" s="163"/>
       <c r="P2" s="164"/>
     </row>
-    <row r="3" spans="1:16" ht="79.2" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:16" ht="81" x14ac:dyDescent="0.9">
       <c r="A3" s="142" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="F3" s="79" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="G3" s="78" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="I3" s="79" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="J3" s="78" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="K3" s="78" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="L3" s="79" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="M3" s="78" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="N3" s="78" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="O3" s="79" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="P3" s="78" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.7">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A4" s="75" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B4" s="61">
         <v>553</v>
@@ -2564,9 +2569,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A5" s="75" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B5" s="61">
         <v>81</v>
@@ -2617,9 +2622,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A6" s="75" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B6" s="61">
         <v>278</v>
@@ -2670,9 +2675,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A7" s="75" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B7" s="61">
         <v>254</v>
@@ -2723,9 +2728,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A8" s="75" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B8" s="59">
         <v>16</v>
@@ -2776,9 +2781,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.9">
       <c r="A9" s="75" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B9" s="61">
         <v>62</v>
@@ -2797,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H9" s="61">
         <v>0</v>
@@ -2806,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="74" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="K9" s="61"/>
       <c r="L9" s="61"/>
@@ -2815,7 +2820,7 @@
       <c r="O9" s="73"/>
       <c r="P9" s="73"/>
     </row>
-    <row r="10" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:16" ht="27.5" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A10" s="72" t="s">
         <v>4</v>
       </c>
@@ -2865,9 +2870,9 @@
         <v>15.203531142717001</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A11" s="67" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2885,7 +2890,7 @@
       <c r="O11" s="155"/>
       <c r="P11" s="155"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.9">
       <c r="O12" s="109"/>
     </row>
   </sheetData>
@@ -2910,19 +2915,19 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="1" customWidth="1"/>
-    <col min="2" max="19" width="11.5546875" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="21.08984375" style="1" customWidth="1"/>
+    <col min="2" max="19" width="11.54296875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A1" s="55" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -2943,68 +2948,68 @@
       <c r="R1" s="56"/>
       <c r="S1" s="56"/>
     </row>
-    <row r="2" spans="1:19" ht="79.2" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:19" ht="81" x14ac:dyDescent="0.9">
       <c r="A2" s="145" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="C2" s="119" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="D2" s="118" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="E2" s="92" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="F2" s="93" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="G2" s="92" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="H2" s="92" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="I2" s="93" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="J2" s="92" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="K2" s="92" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="L2" s="93" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="M2" s="92" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="N2" s="92" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="O2" s="93" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="P2" s="92" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="Q2" s="92" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="R2" s="93" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="S2" s="92" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A3" s="91" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="120">
         <v>403</v>
@@ -3066,9 +3071,9 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A4" s="91" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B4" s="120">
         <v>78</v>
@@ -3130,9 +3135,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A5" s="91" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="120">
         <v>275</v>
@@ -3194,9 +3199,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A6" s="91" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B6" s="120">
         <v>418</v>
@@ -3258,9 +3263,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A7" s="91" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B7" s="122">
         <v>9</v>
@@ -3322,7 +3327,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:19" ht="27.5" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A8" s="88" t="s">
         <v>4</v>
       </c>
@@ -3396,9 +3401,9 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A9" s="84" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B9" s="117"/>
       <c r="C9" s="117"/>
@@ -3411,7 +3416,7 @@
       <c r="J9" s="83"/>
       <c r="K9" s="82"/>
       <c r="L9" s="81" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="M9" s="81"/>
       <c r="N9" s="81"/>
@@ -3421,7 +3426,7 @@
       <c r="R9" s="81"/>
       <c r="S9" s="81"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.9">
       <c r="J10" s="80"/>
     </row>
   </sheetData>
@@ -3438,19 +3443,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="88.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="88.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.36328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:6" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="55" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -3458,7 +3463,7 @@
       <c r="E1" s="55"/>
       <c r="F1" s="55"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.9">
       <c r="A2" s="62" t="s">
         <v>2</v>
       </c>
@@ -3478,9 +3483,9 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A3" s="97" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B3" s="57">
         <v>700</v>
@@ -3498,9 +3503,9 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:6" ht="36.65" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="60" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="B4" s="58">
         <v>1700</v>
@@ -3518,9 +3523,9 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A5" s="60" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5" s="153">
         <v>41.2</v>
@@ -3538,9 +3543,9 @@
         <v>45.946941783345601</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A6" s="96" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="B6" s="96"/>
       <c r="C6" s="96"/>
@@ -3562,18 +3567,18 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="6" width="19.77734375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="6" width="19.81640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:7" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="1">
       <c r="A1" s="55" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="94"/>
@@ -3581,7 +3586,7 @@
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
     </row>
-    <row r="2" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="146"/>
       <c r="B2" s="105">
         <v>2020</v>
@@ -3599,29 +3604,29 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="147" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="104" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="74">
         <v>186.28</v>
@@ -3639,9 +3644,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="104" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B5" s="74">
         <v>60</v>
@@ -3659,9 +3664,9 @@
         <v>86.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A6" s="104" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B6" s="74">
         <v>40</v>
@@ -3679,9 +3684,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A7" s="104" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B7" s="74">
         <v>70.150000000000006</v>
@@ -3699,9 +3704,9 @@
         <v>51.1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" ht="27.5" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A8" s="103" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B8" s="102">
         <v>87.33</v>
@@ -3719,16 +3724,16 @@
         <v>76.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A9" s="100" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B9" s="99"/>
       <c r="D9" s="98"/>
       <c r="E9" s="98"/>
       <c r="F9" s="98"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.9">
       <c r="G10" s="95"/>
     </row>
   </sheetData>
@@ -3745,19 +3750,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="6" width="11.36328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" ht="50.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="165" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="B1" s="165"/>
       <c r="C1" s="165"/>
@@ -3765,9 +3770,9 @@
       <c r="E1" s="165"/>
       <c r="F1" s="165"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.9">
       <c r="A2" s="133" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B2" s="63">
         <v>2010</v>
@@ -3785,9 +3790,9 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.9">
       <c r="A3" s="104" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="B3" s="58">
         <v>1700</v>
@@ -3805,9 +3810,9 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.9">
       <c r="A4" s="108" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B4" s="57">
         <v>62</v>
@@ -3825,9 +3830,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" ht="27.5" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A5" s="107" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B5" s="148">
         <v>3.6470588235294099</v>
@@ -3845,9 +3850,9 @@
         <v>3.01255230125523</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.9">
       <c r="A6" s="106" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B6" s="106"/>
       <c r="C6" s="106"/>
@@ -3869,27 +3874,27 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
     <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.5546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5546875" style="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="4" width="13.54296875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11.54296875" style="1"/>
+    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="166" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="B1" s="166"/>
       <c r="C1" s="166"/>
       <c r="D1" s="166"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A2" s="62" t="s">
         <v>2</v>
       </c>
@@ -3903,9 +3908,9 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A3" s="60" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B3" s="58">
         <v>1328168</v>
@@ -3917,9 +3922,9 @@
         <v>1939342</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A4" s="60" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B4" s="58">
         <v>2957</v>
@@ -3931,9 +3936,9 @@
         <v>4505</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A5" s="60" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B5" s="58">
         <v>749865</v>
@@ -3945,9 +3950,9 @@
         <v>1074208</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A6" s="60" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B6" s="58">
         <v>33200</v>
@@ -3959,9 +3964,9 @@
         <v>53787</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A7" s="60" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B7" s="58">
         <v>10877</v>
@@ -3973,9 +3978,9 @@
         <v>31608</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A8" s="60" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B8" s="58">
         <v>705788</v>
@@ -3987,9 +3992,9 @@
         <v>988822</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A9" s="125" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B9" s="149">
         <v>56.5</v>
@@ -4001,24 +4006,24 @@
         <v>55.39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A10" s="9" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.9">
       <c r="D13" s="124"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.9">
       <c r="D14" s="124"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.9">
       <c r="D15" s="124"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.7">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.9">
       <c r="D17" s="124"/>
     </row>
   </sheetData>
@@ -4035,25 +4040,25 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="14.77734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="25.90625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="14.81640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:7" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:7" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A2" s="33" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -4062,23 +4067,23 @@
       <c r="F2" s="128"/>
       <c r="G2" s="127"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="140" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.7">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A4" s="97" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="B4" s="58">
         <v>147</v>
@@ -4090,9 +4095,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="97" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="B5" s="58">
         <v>37</v>
@@ -4105,9 +4110,9 @@
       </c>
       <c r="F5" s="126"/>
     </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A6" s="97" t="s">
-        <v>75</v>
+        <v>173</v>
       </c>
       <c r="B6" s="150">
         <v>25.170068027210899</v>
@@ -4119,9 +4124,9 @@
         <v>26.751592356687901</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A7" s="167" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B7" s="167"/>
       <c r="C7" s="167"/>
@@ -4141,28 +4146,28 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.90625" style="1" customWidth="1"/>
     <col min="2" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="1"/>
+    <col min="5" max="5" width="13.1796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="33" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A2" s="133" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B2" s="132">
         <v>2013</v>
@@ -4174,9 +4179,9 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A3" s="131" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B3" s="130">
         <v>1189105</v>
@@ -4188,9 +4193,9 @@
         <v>1786448</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A4" s="131" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" s="130">
         <v>898100</v>
@@ -4202,9 +4207,9 @@
         <v>1272837</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A5" s="131" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B5" s="130">
         <v>147</v>
@@ -4216,9 +4221,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A6" s="131" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B6" s="130">
         <v>64</v>
@@ -4230,9 +4235,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A7" s="131" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B7" s="130">
         <v>438</v>
@@ -4244,9 +4249,9 @@
         <v>559</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A8" s="129" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B8" s="151">
         <v>75.53</v>
@@ -4258,9 +4263,9 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A9" s="167" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B9" s="167"/>
       <c r="C9" s="9"/>
@@ -4279,28 +4284,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF716CA6-EB93-4872-A88E-E3E7686AD6A1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="13.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="31.90625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="13.90625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="33" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A2" s="62" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B2" s="29">
         <v>2013</v>
@@ -4312,9 +4315,9 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A3" s="135" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B3" s="58">
         <v>1189105</v>
@@ -4326,9 +4329,9 @@
         <v>1786448</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A4" s="135" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" s="58">
         <v>898100</v>
@@ -4340,9 +4343,9 @@
         <v>1272837</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A5" s="135" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B5" s="58">
         <v>147</v>
@@ -4354,9 +4357,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A6" s="135" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B6" s="58">
         <v>64</v>
@@ -4368,9 +4371,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A7" s="135" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B7" s="58">
         <v>438</v>
@@ -4382,9 +4385,9 @@
         <v>559</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A8" s="134" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B8" s="152">
         <v>0.75529999999999997</v>
@@ -4396,9 +4399,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.9">
       <c r="A9" s="168" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B9" s="168"/>
       <c r="C9" s="9"/>
@@ -4420,19 +4423,19 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="2" width="18.21875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="9.5546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="18.1796875" style="1" customWidth="1"/>
+    <col min="3" max="7" width="9.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:7" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="15" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="8"/>
@@ -4441,7 +4444,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -4464,7 +4467,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
@@ -4487,7 +4490,7 @@
         <v>4312</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -4510,7 +4513,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>7098</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -4555,26 +4558,26 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="31.453125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.08984375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:3" s="82" customFormat="1" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="137" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
       <c r="B1" s="138"/>
       <c r="C1" s="138"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A2" s="62" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B2" s="29">
         <v>2018</v>
@@ -4583,9 +4586,9 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A3" s="136" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B3" s="58">
         <v>1417823</v>
@@ -4594,9 +4597,9 @@
         <v>1786448</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A4" s="97" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" s="58">
         <v>1041199</v>
@@ -4605,9 +4608,9 @@
         <v>1272837</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A5" s="97" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B5" s="58">
         <v>800379</v>
@@ -4616,9 +4619,9 @@
         <v>1255463</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A6" s="97" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B6" s="58">
         <v>219670</v>
@@ -4627,9 +4630,9 @@
         <v>255615</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A7" s="97" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B7" s="152">
         <v>73</v>
@@ -4638,9 +4641,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.9">
       <c r="A8" s="168" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B8" s="168"/>
       <c r="C8" s="9"/>
@@ -4649,20 +4652,6 @@
   <mergeCells count="1">
     <mergeCell ref="A8:B8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFFBB71-181B-402D-A1DB-DF08982905F0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4675,19 +4664,19 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="2" width="21.21875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="11.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="21.1796875" style="1" customWidth="1"/>
+    <col min="3" max="7" width="11.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:8" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="15" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="8"/>
@@ -4696,7 +4685,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.9">
       <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
@@ -4719,7 +4708,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.9">
       <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
@@ -4742,7 +4731,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.9">
       <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
@@ -4765,7 +4754,7 @@
         <v>5064</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.9">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
@@ -4788,7 +4777,7 @@
         <v>7098</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.9">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -4813,19 +4802,19 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="2" width="16.109375" style="1" customWidth="1"/>
+    <col min="1" max="2" width="16.08984375" style="1" customWidth="1"/>
     <col min="3" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="8" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:7" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="15" t="s">
-        <v>14</v>
+        <v>155</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="8"/>
@@ -4834,7 +4823,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
@@ -4857,7 +4846,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
@@ -4880,7 +4869,7 @@
         <v>74534</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -4903,7 +4892,7 @@
         <v>80611</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -4926,7 +4915,7 @@
         <v>155145</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -4950,18 +4939,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="21.36328125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:7" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="15" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="8"/>
@@ -4970,7 +4959,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
@@ -4993,7 +4982,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
@@ -5016,7 +5005,7 @@
         <v>73602</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="22.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -5039,7 +5028,7 @@
         <v>81603</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -5062,7 +5051,7 @@
         <v>155205</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.9">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -5082,18 +5071,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB79EA6F-52D8-4271-9F0B-1B8DE97AB912}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -5105,7 +5094,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
@@ -5137,9 +5126,9 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="31">
         <v>12</v>
@@ -5169,9 +5158,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="27" t="s">
-        <v>17</v>
+        <v>158</v>
       </c>
       <c r="B4" s="32">
         <v>0.47</v>
@@ -5201,7 +5190,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
         <v>11</v>
       </c>
@@ -5216,18 +5205,18 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="11" width="20.109375" style="45" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="11" width="20.08984375" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="33" t="s">
-        <v>18</v>
+        <v>159</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -5240,44 +5229,44 @@
       <c r="J1" s="43"/>
       <c r="K1" s="43"/>
     </row>
-    <row r="2" spans="1:11" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="108" x14ac:dyDescent="0.35">
       <c r="A2" s="139" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="54" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="46">
         <v>1</v>
@@ -5310,9 +5299,9 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="52.8" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.9">
       <c r="A4" s="39" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" s="46">
         <v>1</v>
@@ -5345,9 +5334,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="46">
         <v>2</v>
@@ -5380,9 +5369,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="46">
         <v>1</v>
@@ -5415,9 +5404,9 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="46">
         <v>1</v>
@@ -5450,9 +5439,9 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="46">
         <v>2</v>
@@ -5485,9 +5474,9 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="46">
         <v>0</v>
@@ -5520,9 +5509,9 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="81" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="46">
         <v>5</v>
@@ -5555,9 +5544,9 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" s="46">
         <v>1</v>
@@ -5590,9 +5579,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="54" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="46">
         <v>1</v>
@@ -5625,9 +5614,9 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="54" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" s="46">
         <v>0</v>
@@ -5660,9 +5649,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" s="46">
         <v>0</v>
@@ -5695,9 +5684,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="46">
         <v>14</v>
@@ -5728,9 +5717,9 @@
       </c>
       <c r="K15" s="37"/>
     </row>
-    <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="27" x14ac:dyDescent="0.35">
       <c r="A16" s="35" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="47">
         <v>29</v>
@@ -5763,7 +5752,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.7">
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
@@ -5790,35 +5779,35 @@
   </sheetPr>
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="1" width="59.88671875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.90625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="11.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.5546875" style="1"/>
+    <col min="20" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:19" ht="29.5" x14ac:dyDescent="0.95">
       <c r="A1" s="55" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -5839,74 +5828,74 @@
       <c r="R1" s="54"/>
       <c r="S1" s="54"/>
     </row>
-    <row r="2" spans="1:19" ht="52.8" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:19" ht="54" x14ac:dyDescent="0.9">
       <c r="A2" s="139" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="R2" s="34" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A3" s="36" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="51">
         <v>73</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D3" s="51">
         <v>73</v>
@@ -5915,7 +5904,7 @@
         <v>73</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G3" s="51">
         <v>73</v>
@@ -5924,7 +5913,7 @@
         <v>77</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J3" s="51">
         <v>77</v>
@@ -5933,7 +5922,7 @@
         <v>89</v>
       </c>
       <c r="L3" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M3" s="51">
         <v>89</v>
@@ -5942,7 +5931,7 @@
         <v>79</v>
       </c>
       <c r="O3" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P3" s="51">
         <v>79</v>
@@ -5957,15 +5946,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A4" s="39" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" s="51">
         <v>41</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D4" s="51">
         <v>41</v>
@@ -5974,7 +5963,7 @@
         <v>41</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G4" s="51">
         <v>41</v>
@@ -5983,7 +5972,7 @@
         <v>34</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J4" s="51">
         <v>34</v>
@@ -5992,7 +5981,7 @@
         <v>41</v>
       </c>
       <c r="L4" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M4" s="51">
         <v>41</v>
@@ -6001,7 +5990,7 @@
         <v>30</v>
       </c>
       <c r="O4" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P4" s="51">
         <v>30</v>
@@ -6016,15 +6005,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A5" s="36" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="51">
         <v>55</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D5" s="51">
         <v>55</v>
@@ -6033,7 +6022,7 @@
         <v>55</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G5" s="51">
         <v>55</v>
@@ -6042,7 +6031,7 @@
         <v>54</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J5" s="51">
         <v>54</v>
@@ -6051,7 +6040,7 @@
         <v>54</v>
       </c>
       <c r="L5" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M5" s="51">
         <v>54</v>
@@ -6060,7 +6049,7 @@
         <v>52</v>
       </c>
       <c r="O5" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P5" s="51">
         <v>52</v>
@@ -6075,15 +6064,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A6" s="36" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="51">
         <v>31</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D6" s="51">
         <v>31</v>
@@ -6092,7 +6081,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G6" s="51">
         <v>31</v>
@@ -6101,7 +6090,7 @@
         <v>29</v>
       </c>
       <c r="I6" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J6" s="51">
         <v>29</v>
@@ -6110,7 +6099,7 @@
         <v>34</v>
       </c>
       <c r="L6" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M6" s="51">
         <v>34</v>
@@ -6119,7 +6108,7 @@
         <v>37</v>
       </c>
       <c r="O6" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P6" s="51">
         <v>37</v>
@@ -6134,15 +6123,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A7" s="36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="51">
         <v>335</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D7" s="51">
         <v>335</v>
@@ -6151,7 +6140,7 @@
         <v>335</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G7" s="51">
         <v>335</v>
@@ -6160,7 +6149,7 @@
         <v>457</v>
       </c>
       <c r="I7" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J7" s="51">
         <v>457</v>
@@ -6169,7 +6158,7 @@
         <v>354</v>
       </c>
       <c r="L7" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M7" s="51">
         <v>354</v>
@@ -6178,7 +6167,7 @@
         <v>268</v>
       </c>
       <c r="O7" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P7" s="51">
         <v>268</v>
@@ -6193,15 +6182,15 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A8" s="36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="51">
         <v>40</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" s="51">
         <v>40</v>
@@ -6210,7 +6199,7 @@
         <v>57</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G8" s="51">
         <v>57</v>
@@ -6219,7 +6208,7 @@
         <v>57</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J8" s="51">
         <v>57</v>
@@ -6228,7 +6217,7 @@
         <v>82</v>
       </c>
       <c r="L8" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M8" s="51">
         <v>82</v>
@@ -6237,7 +6226,7 @@
         <v>57</v>
       </c>
       <c r="O8" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P8" s="51">
         <v>57</v>
@@ -6252,15 +6241,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A9" s="36" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="51">
         <v>5</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D9" s="51">
         <v>5</v>
@@ -6269,7 +6258,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G9" s="51">
         <v>8</v>
@@ -6278,7 +6267,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J9" s="51">
         <v>18</v>
@@ -6287,7 +6276,7 @@
         <v>14</v>
       </c>
       <c r="L9" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M9" s="51">
         <v>14</v>
@@ -6296,7 +6285,7 @@
         <v>14</v>
       </c>
       <c r="O9" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P9" s="51">
         <v>14</v>
@@ -6311,9 +6300,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="23.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:19" ht="23.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A10" s="36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="51">
         <v>427</v>
@@ -6355,7 +6344,7 @@
         <v>312</v>
       </c>
       <c r="O10" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P10" s="51">
         <v>312</v>
@@ -6370,15 +6359,15 @@
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A11" s="36" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" s="51">
         <v>4</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D11" s="51">
         <v>4</v>
@@ -6387,7 +6376,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G11" s="51">
         <v>4</v>
@@ -6396,7 +6385,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J11" s="51">
         <v>4</v>
@@ -6405,7 +6394,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M11" s="51">
         <v>6</v>
@@ -6414,7 +6403,7 @@
         <v>178</v>
       </c>
       <c r="O11" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P11" s="51">
         <v>178</v>
@@ -6429,15 +6418,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A12" s="36" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="51">
         <v>60</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D12" s="51">
         <v>60</v>
@@ -6446,7 +6435,7 @@
         <v>60</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G12" s="51">
         <v>60</v>
@@ -6455,7 +6444,7 @@
         <v>60</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J12" s="51">
         <v>60</v>
@@ -6464,7 +6453,7 @@
         <v>57</v>
       </c>
       <c r="L12" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M12" s="51">
         <v>57</v>
@@ -6473,7 +6462,7 @@
         <v>54</v>
       </c>
       <c r="O12" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P12" s="51">
         <v>54</v>
@@ -6488,15 +6477,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A13" s="36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" s="51">
         <v>35</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D13" s="51">
         <v>35</v>
@@ -6505,7 +6494,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G13" s="51">
         <v>18</v>
@@ -6514,7 +6503,7 @@
         <v>32</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J13" s="51">
         <v>32</v>
@@ -6523,7 +6512,7 @@
         <v>18</v>
       </c>
       <c r="L13" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M13" s="51">
         <v>18</v>
@@ -6532,7 +6521,7 @@
         <v>13</v>
       </c>
       <c r="O13" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P13" s="51">
         <v>13</v>
@@ -6547,15 +6536,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A14" s="36" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" s="51">
         <v>5</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D14" s="51">
         <v>5</v>
@@ -6564,7 +6553,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G14" s="51">
         <v>4</v>
@@ -6573,7 +6562,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J14" s="51">
         <v>4</v>
@@ -6582,7 +6571,7 @@
         <v>16</v>
       </c>
       <c r="L14" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M14" s="51">
         <v>16</v>
@@ -6591,7 +6580,7 @@
         <v>7</v>
       </c>
       <c r="O14" s="51" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P14" s="51">
         <v>7</v>
@@ -6606,9 +6595,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A15" s="36" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="51">
         <v>760</v>
@@ -6665,9 +6654,9 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A16" s="35" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="52">
         <v>1871</v>
@@ -6724,9 +6713,9 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A17" s="50" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -6735,7 +6724,7 @@
       <c r="F17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A18" s="49"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -6744,12 +6733,12 @@
       <c r="F18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="35" ht="18.75" customHeight="1" x14ac:dyDescent="0.7"/>
-    <row r="36" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.7"/>
-    <row r="47" ht="18" customHeight="1" x14ac:dyDescent="0.7"/>
-    <row r="48" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.7"/>
-    <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.7"/>
-    <row r="68" ht="18" customHeight="1" x14ac:dyDescent="0.7"/>
+    <row r="35" ht="18.75" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="36" ht="37.75" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="47" ht="18" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="48" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="68" ht="18" customHeight="1" x14ac:dyDescent="0.9"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6764,18 +6753,18 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="26.4" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="27" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="19" width="17.44140625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="19" width="17.453125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="22.8" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A1" s="64" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -6796,68 +6785,68 @@
       <c r="R1" s="64"/>
       <c r="S1" s="64"/>
     </row>
-    <row r="2" spans="1:19" ht="52.8" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:19" ht="54" x14ac:dyDescent="0.9">
       <c r="A2" s="140" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="110" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="C2" s="111" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="Q2" s="34" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="R2" s="34" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="S2" s="34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A3" s="60" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="112">
         <v>760</v>
@@ -6871,7 +6860,7 @@
         <v>609</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G3" s="58">
         <v>609</v>
@@ -6880,7 +6869,7 @@
         <v>935</v>
       </c>
       <c r="I3" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J3" s="57">
         <v>935</v>
@@ -6889,7 +6878,7 @@
         <v>1039</v>
       </c>
       <c r="L3" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M3" s="58">
         <v>1039</v>
@@ -6898,7 +6887,7 @@
         <v>1017</v>
       </c>
       <c r="O3" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P3" s="58">
         <v>1017</v>
@@ -6913,9 +6902,9 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A4" s="60" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B4" s="112">
         <v>102</v>
@@ -6929,7 +6918,7 @@
         <v>84</v>
       </c>
       <c r="F4" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G4" s="58">
         <v>84</v>
@@ -6938,7 +6927,7 @@
         <v>108</v>
       </c>
       <c r="I4" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J4" s="57">
         <v>108</v>
@@ -6947,7 +6936,7 @@
         <v>115</v>
       </c>
       <c r="L4" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M4" s="58">
         <v>115</v>
@@ -6956,7 +6945,7 @@
         <v>108</v>
       </c>
       <c r="O4" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P4" s="58">
         <v>108</v>
@@ -6971,9 +6960,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A5" s="60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="112">
         <v>422</v>
@@ -7016,7 +7005,7 @@
         <v>312</v>
       </c>
       <c r="O5" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P5" s="58">
         <v>312</v>
@@ -7031,9 +7020,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A6" s="60" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B6" s="112">
         <v>589</v>
@@ -7047,7 +7036,7 @@
         <v>288</v>
       </c>
       <c r="F6" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G6" s="58">
         <v>288</v>
@@ -7056,7 +7045,7 @@
         <v>444</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J6" s="57">
         <v>444</v>
@@ -7065,7 +7054,7 @@
         <v>221</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="M6" s="58">
         <v>221</v>
@@ -7074,7 +7063,7 @@
         <v>268</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P6" s="58">
         <v>268</v>
@@ -7089,9 +7078,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.9">
       <c r="A7" s="60" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B7" s="115">
         <v>0</v>
@@ -7149,9 +7138,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A8" s="50" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>

</xml_diff>